<commit_message>
Doc: Changed doc + logbook
</commit_message>
<xml_diff>
--- a/docs/Logbook.xlsx
+++ b/docs/Logbook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t xml:space="preserve">Don’t remove python 3.6 from ubuntu!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setting up YOLO</t>
   </si>
 </sst>
 </file>
@@ -251,10 +254,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -461,6 +464,19 @@
       <c r="A18" s="4" t="n">
         <v>43747</v>
       </c>
+      <c r="B18" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="n">
+        <v>43774</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="n">
+        <v>43775</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Doc: updated logbook + added notes file
</commit_message>
<xml_diff>
--- a/docs/Logbook.xlsx
+++ b/docs/Logbook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t xml:space="preserve">Realsense-ROS version 2.2.9 | Realsense SDK version 2.29.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed ROS with Realsense SDK, started ROS research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finished getTF, updated class diagram</t>
   </si>
 </sst>
 </file>
@@ -302,7 +308,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -587,6 +593,12 @@
       <c r="A24" s="4" t="n">
         <v>43782</v>
       </c>
+      <c r="B24" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Doc: Updated logbook and added docs
</commit_message>
<xml_diff>
--- a/docs/Logbook.xlsx
+++ b/docs/Logbook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -215,6 +215,15 @@
   </si>
   <si>
     <t xml:space="preserve">test data is saved in .csv file that is in the build folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrated pipeline into ROS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed client service with images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrated client service into main</t>
   </si>
 </sst>
 </file>
@@ -338,10 +347,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -686,6 +695,35 @@
         <v>64</v>
       </c>
     </row>
+    <row r="29" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="n">
+        <v>43798</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="n">
+        <v>43801</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="n">
+        <v>43802</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="n">
+        <v>43803</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Fix: code ready for testing
</commit_message>
<xml_diff>
--- a/docs/Logbook.xlsx
+++ b/docs/Logbook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -236,6 +236,15 @@
   </si>
   <si>
     <t xml:space="preserve">cv_bridge doesn’ t work with python3, yolo only works with python3. We chose to use a communication protocol made by Merian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research YOLO in C++</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Started documentation + visitation company for robohub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yolo is not in c++ without wrapper so we stay with the yolo we currently use and fix the communication with Marian</t>
   </si>
 </sst>
 </file>
@@ -359,7 +368,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
@@ -747,6 +756,25 @@
       <c r="A32" s="4" t="n">
         <v>43803</v>
       </c>
+      <c r="B32" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="n">
+        <v>43809</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="n">
+        <v>43810</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
doc: updated docs and logbook
</commit_message>
<xml_diff>
--- a/docs/Logbook.xlsx
+++ b/docs/Logbook.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="82">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t xml:space="preserve">Integrating cut_filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing, processing test data and working on documentation</t>
   </si>
 </sst>
 </file>
@@ -274,7 +277,7 @@
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -305,6 +308,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -348,7 +357,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -367,6 +376,10 @@
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -389,7 +402,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -829,6 +842,12 @@
       <c r="A37" s="4" t="n">
         <v>43817</v>
       </c>
+      <c r="B37" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>